<commit_message>
split properness and respectfulness
</commit_message>
<xml_diff>
--- a/thesis-tex/excels/todo.xlsx
+++ b/thesis-tex/excels/todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5555F19C-EBFD-4C9F-9DA4-AF808C9BA93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2493E6-2977-4F48-AB46-823A63340B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5E98CAFA-3C68-43D4-B8FA-5BDF0312E4FD}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="82">
   <si>
     <t>Graphics</t>
   </si>
@@ -255,9 +255,6 @@
     <t>cite theorems in the name</t>
   </si>
   <si>
-    <t>appendix?</t>
-  </si>
-  <si>
     <t>Make figures higher res / same font</t>
   </si>
   <si>
@@ -267,13 +264,25 @@
     <t>MASKIN NOTES</t>
   </si>
   <si>
-    <t>GLICK NOTES</t>
-  </si>
-  <si>
     <t>PAPER NOTES</t>
   </si>
   <si>
     <t>references with volumes, capitatlization, etc?</t>
+  </si>
+  <si>
+    <t>GLICK NOTES [[INDEX]]</t>
+  </si>
+  <si>
+    <t>appendix?/index</t>
+  </si>
+  <si>
+    <t>$$$$ for signatures</t>
+  </si>
+  <si>
+    <t>can figures have the same name</t>
+  </si>
+  <si>
+    <t>capitalize in figure names?</t>
   </si>
 </sst>
 </file>
@@ -353,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -367,6 +376,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,7 +694,7 @@
   <dimension ref="B3:O69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -972,7 +982,7 @@
         <v>12</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J12" t="s">
         <v>12</v>
@@ -994,7 +1004,7 @@
         <v>12</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4" t="s">
@@ -1004,7 +1014,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J13" t="s">
         <v>12</v>
@@ -1034,7 +1044,7 @@
         <v>12</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J14" t="s">
         <v>12</v>
@@ -1142,7 +1152,9 @@
       <c r="B19" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="1"/>
+      <c r="G19" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="H19" t="s">
         <v>12</v>
       </c>
@@ -1163,7 +1175,7 @@
         <v>12</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="H20" t="s">
         <v>12</v>
@@ -1184,6 +1196,9 @@
       <c r="B21" t="s">
         <v>12</v>
       </c>
+      <c r="G21" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="H21" t="s">
         <v>12</v>
       </c>
@@ -1202,6 +1217,9 @@
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>12</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="H22" t="s">
         <v>12</v>
@@ -1531,7 +1549,7 @@
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.3">
       <c r="G4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.3">
@@ -1566,7 +1584,7 @@
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.3">
       <c r="G11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="4:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
multibracket initial sweep (174 pounds)
</commit_message>
<xml_diff>
--- a/thesis-tex/excels/todo.xlsx
+++ b/thesis-tex/excels/todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E87E6E-BB91-4B30-B3F4-FB27713E2501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4C12DE-BEC9-4EE6-BD26-9687F6135B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5E98CAFA-3C68-43D4-B8FA-5BDF0312E4FD}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="89">
   <si>
     <t>Graphics</t>
   </si>
@@ -252,12 +252,6 @@
     <t>cite theorems in the name</t>
   </si>
   <si>
-    <t>Make figures higher res / same font</t>
-  </si>
-  <si>
-    <t>where to put commas, ands, and bullets vs numbers for lists in definitions, itemize vs enumerate</t>
-  </si>
-  <si>
     <t>MASKIN NOTES</t>
   </si>
   <si>
@@ -283,6 +277,33 @@
   </si>
   <si>
     <t>chapter headings should have TOC</t>
+  </si>
+  <si>
+    <t>Add dashed lines where appropiate</t>
+  </si>
+  <si>
+    <t>Wordchoice</t>
+  </si>
+  <si>
+    <t>More</t>
+  </si>
+  <si>
+    <t>lists</t>
+  </si>
+  <si>
+    <t>adjective definitions</t>
+  </si>
+  <si>
+    <t>glossery thing</t>
+  </si>
+  <si>
+    <t>p+r</t>
+  </si>
+  <si>
+    <t>cite the sports leagues (and taladega nights, P-I naming, nba playing why, zurish swiss, others) when I use them</t>
+  </si>
+  <si>
+    <t>zurich switzerland</t>
   </si>
 </sst>
 </file>
@@ -362,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -376,6 +397,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,7 +716,7 @@
   <dimension ref="B3:O69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -849,8 +872,8 @@
       <c r="D8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>23</v>
+      <c r="E8" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
@@ -881,12 +904,12 @@
       <c r="D9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>50</v>
+      <c r="E9" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H9" t="s">
         <v>12</v>
@@ -912,7 +935,7 @@
         <v>12</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4" t="s">
@@ -942,7 +965,7 @@
         <v>12</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4" t="s">
@@ -971,7 +994,7 @@
         <v>12</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4" t="s">
@@ -981,7 +1004,7 @@
         <v>12</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J12" t="s">
         <v>12</v>
@@ -1003,7 +1026,7 @@
         <v>12</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4" t="s">
@@ -1013,7 +1036,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J13" t="s">
         <v>12</v>
@@ -1034,8 +1057,8 @@
       <c r="D14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>48</v>
+      <c r="E14" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="5" t="s">
@@ -1045,7 +1068,7 @@
         <v>12</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J14" t="s">
         <v>12</v>
@@ -1060,14 +1083,14 @@
       <c r="B15" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="7" t="s">
         <v>62</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>80</v>
+      <c r="E15" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4" t="s">
@@ -1093,7 +1116,9 @@
       <c r="D16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="F16" s="4"/>
       <c r="G16" s="5" t="s">
         <v>67</v>
@@ -1136,7 +1161,7 @@
         <v>12</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H18" t="s">
         <v>12</v>
@@ -1156,7 +1181,7 @@
         <v>12</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H19" t="s">
         <v>12</v>
@@ -1197,7 +1222,7 @@
         <v>12</v>
       </c>
       <c r="G21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H21" t="s">
         <v>12</v>
@@ -1530,62 +1555,149 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7103E2D-1F50-4993-9D81-162BA3E4B70C}">
-  <dimension ref="C3:G18"/>
+  <dimension ref="B3:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="79.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="G4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="G5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="G6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="G7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="G8" t="s">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="G9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="G10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="G11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D18" s="1"/>
+      <c r="E6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="13"/>
+      <c r="D8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D9" s="13"/>
+      <c r="E9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D10" s="13"/>
+      <c r="E10" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D11" s="13"/>
+      <c r="E11" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D12" s="13"/>
+      <c r="E12" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D13" s="13"/>
+      <c r="E13" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D14" s="13"/>
+      <c r="E14" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D15" s="13"/>
+      <c r="E15" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D16" s="13"/>
+      <c r="E16" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
re-up intro for nee
</commit_message>
<xml_diff>
--- a/thesis-tex/excels/todo.xlsx
+++ b/thesis-tex/excels/todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4C12DE-BEC9-4EE6-BD26-9687F6135B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71A203E-8A2C-4B3C-A288-B547B64E08C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5E98CAFA-3C68-43D4-B8FA-5BDF0312E4FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{5E98CAFA-3C68-43D4-B8FA-5BDF0312E4FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="86">
   <si>
     <t>Graphics</t>
   </si>
@@ -279,31 +279,22 @@
     <t>chapter headings should have TOC</t>
   </si>
   <si>
-    <t>Add dashed lines where appropiate</t>
-  </si>
-  <si>
-    <t>Wordchoice</t>
-  </si>
-  <si>
     <t>More</t>
   </si>
   <si>
-    <t>lists</t>
-  </si>
-  <si>
-    <t>adjective definitions</t>
-  </si>
-  <si>
     <t>glossery thing</t>
   </si>
   <si>
-    <t>p+r</t>
-  </si>
-  <si>
-    <t>cite the sports leagues (and taladega nights, P-I naming, nba playing why, zurish swiss, others) when I use them</t>
-  </si>
-  <si>
     <t>zurich switzerland</t>
+  </si>
+  <si>
+    <t>swiss, p + r, intro</t>
+  </si>
+  <si>
+    <t>sort thru sheet1</t>
+  </si>
+  <si>
+    <t>cite the sports leagues (and taladega nights, P-I naming, nba playing why, zurish swiss, others) when I use them and also cite SST inventor</t>
   </si>
 </sst>
 </file>
@@ -383,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -398,7 +389,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -715,7 +705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD8268EF-D185-4740-9164-A0FF02A9F021}">
   <dimension ref="B3:O69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -873,7 +863,7 @@
         <v>12</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
@@ -1555,149 +1545,86 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7103E2D-1F50-4993-9D81-162BA3E4B70C}">
-  <dimension ref="B3:F21"/>
+  <dimension ref="B4:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="35.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.88671875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="13"/>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B6" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B8" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B9" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B10" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="13"/>
-      <c r="D8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D9" s="13"/>
-      <c r="E9" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D10" s="13"/>
-      <c r="E10" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D11" s="13"/>
-      <c r="E11" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D12" s="13"/>
-      <c r="E12" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D13" s="13"/>
-      <c r="E13" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D14" s="13"/>
-      <c r="E14" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D15" s="13"/>
-      <c r="E15" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D16" s="13"/>
-      <c r="E16" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-    </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-    </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-    </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B12" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B13" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B14" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B15" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B16" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="13"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="13"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="13"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="13"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
swiss as flowcharts and start of refs
</commit_message>
<xml_diff>
--- a/thesis-tex/excels/todo.xlsx
+++ b/thesis-tex/excels/todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71A203E-8A2C-4B3C-A288-B547B64E08C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1648E8-FDB6-4C55-8B60-2728012531FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{5E98CAFA-3C68-43D4-B8FA-5BDF0312E4FD}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="88">
   <si>
     <t>Graphics</t>
   </si>
@@ -294,7 +294,13 @@
     <t>sort thru sheet1</t>
   </si>
   <si>
-    <t>cite the sports leagues (and taladega nights, P-I naming, nba playing why, zurish swiss, others) when I use them and also cite SST inventor</t>
+    <t>but randomization figures in the proof</t>
+  </si>
+  <si>
+    <t>(nee orderedness/edwardsian/(reseed [disproof more and also c.e better]) comments)</t>
+  </si>
+  <si>
+    <t>cite the sports leagues (and taladega nights, mtg swiss P-I naming, nba playing why, nfl expansion, zurish swiss, others) when I use them and also cite SST inventor</t>
   </si>
 </sst>
 </file>
@@ -374,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -388,7 +394,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1545,25 +1550,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7103E2D-1F50-4993-9D81-162BA3E4B70C}">
-  <dimension ref="B4:B21"/>
+  <dimension ref="B5:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B4" s="13"/>
-    </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
-        <v>85</v>
+      <c r="B6" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.3">
@@ -1572,59 +1574,49 @@
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B8" s="13" t="s">
+      <c r="B8" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B9" s="13" t="s">
+      <c r="B9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B10" s="13" t="s">
+      <c r="B10" t="s">
         <v>83</v>
       </c>
     </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+    </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B12" s="13" t="s">
-        <v>12</v>
+      <c r="B12" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B13" s="13" t="s">
+      <c r="B13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B14" s="13" t="s">
+      <c r="B14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B15" s="13" t="s">
+      <c r="B15" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B16" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" s="13"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" s="13"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B19" s="13"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" s="13"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B21" s="13"/>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
lots of glossary work
</commit_message>
<xml_diff>
--- a/thesis-tex/excels/todo.xlsx
+++ b/thesis-tex/excels/todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916D063D-F63F-4E70-9F4D-5F643C71C659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C46F84-7195-484B-846C-6CAD46E7FF0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{5E98CAFA-3C68-43D4-B8FA-5BDF0312E4FD}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="133">
   <si>
     <t>Graphics</t>
   </si>
@@ -377,9 +377,6 @@
     <t>Think about containment and exciting definitions</t>
   </si>
   <si>
-    <t>Move randomness figures into proof</t>
-  </si>
-  <si>
     <t>Multibrackets</t>
   </si>
   <si>
@@ -389,9 +386,6 @@
     <t>Postmatter</t>
   </si>
   <si>
-    <t>Glossery for chapters 1 and 3</t>
-  </si>
-  <si>
     <t>Format glossery</t>
   </si>
   <si>
@@ -410,9 +404,6 @@
     <t>last %s</t>
   </si>
   <si>
-    <t>proofs and defs with person/year</t>
-  </si>
-  <si>
     <t>exp to swiss</t>
   </si>
   <si>
@@ -435,6 +426,18 @@
   </si>
   <si>
     <t>think about printing</t>
+  </si>
+  <si>
+    <t>proofs and defs with person/year + conjs + corrs + get rid of talking about it hten</t>
+  </si>
+  <si>
+    <t>Move randomness + E.T. figures into proof</t>
+  </si>
+  <si>
+    <t>determine who defined and proved simple things</t>
+  </si>
+  <si>
+    <t>Glossery for chapters 1 and 3 and nameed theos</t>
   </si>
 </sst>
 </file>
@@ -1958,10 +1961,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83C5A7EC-BEB1-4B41-B6F6-3FA523223DFE}">
-  <dimension ref="B5:J10"/>
+  <dimension ref="B5:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1981,13 +1984,13 @@
         <v>108</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
@@ -1998,13 +2001,13 @@
         <v>109</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H6" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="J6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
@@ -2015,13 +2018,13 @@
         <v>110</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
@@ -2032,13 +2035,13 @@
         <v>111</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="H8" t="s">
-        <v>123</v>
+        <v>121</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>129</v>
       </c>
       <c r="J8" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
@@ -2046,16 +2049,16 @@
         <v>105</v>
       </c>
       <c r="D9" t="s">
-        <v>112</v>
-      </c>
-      <c r="F9" t="s">
-        <v>129</v>
+        <v>130</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>126</v>
       </c>
       <c r="H9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
@@ -2063,16 +2066,21 @@
         <v>107</v>
       </c>
       <c r="D10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F10" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J10" t="s">
-        <v>121</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>